<commit_message>
Added detail, clean-up layout.
detail schema & logo clean-up
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t xml:space="preserve">in_resume</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">Something smart.</t>
   </si>
   <si>
+    <t xml:space="preserve">summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Head of Development</t>
   </si>
   <si>
@@ -94,28 +97,85 @@
     <t xml:space="preserve">MSD Capital, L.P.</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Lead</t>
+    <t xml:space="preserve">Quantitative Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promontory Financial Group</t>
   </si>
   <si>
     <t xml:space="preserve">Senior Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">Head of data mining project to establish temporal trends in population densities of Mysis diluviana (Mysis).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ran project to mathematically model the migration patterns of Mysis (honors thesis project.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description_5</t>
+    <t xml:space="preserve">Charlotte, NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RR Donnelley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">technology</t>
   </si>
   <si>
     <t xml:space="preserve">Analytics Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead development effort on our in-house proprietary data analytics  and risk system on a team of five.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation layer constructed with WPF/C#, Service-Oriented-Architecture built with WCF/C#, data layer modeled in T-SQL and processed with R packages deployed to the server instance, invoked directly with stored procedures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Built a suite of FX hedging and settlement tools to automate our FX process. Constructed the core FX Hedging model in R, which used various metrics of hedging (FMV, Cost, MTM, Fixed, Underlying, Custom Model, etc.) to calculate the target hedge by strategy then aggregate by total currency exposure across the firm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build multiple factor-based models in R leveraging Bloomberg data for the India market working directly with the portfolio manager through various iterations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Built a real-time Profit-Loss system by integrating data from our core accounting / OMS systems, then enriching the data sets with market data using our proprietary Market Data service build in WCF using RX/C#.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R, C#, WPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option Pricing Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed a custom in-house option-pricing framework that involved leveraging QuantLib (an open source C++ financial library) for the derivative pricing engine and adding functionality that generated a variance/underlying "shock matrix" for a given option.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed a WPF application style with a custom configurable n x m matrix data layout (for the pricing matrix), along with custom data overlays in each cell when pricing a strategy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed a reusable Bloomberg Data Module for the SAPI API that was responsible for pulling option-pricing parameters (underlying, strike, volatility, maturity date, risk-free rate and dividend yield) in real-time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++, C#, WPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independent Foreclosure Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RightContent</t>
   </si>
   <si>
     <t xml:space="preserve">skill</t>
@@ -152,10 +212,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -221,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,6 +297,18 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -372,10 +445,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -386,10 +459,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="168.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="87.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="75.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="55.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="168.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="87.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="75.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,13 +486,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,26 +494,19 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>42736</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>43800</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>23</v>
-      </c>
+        <v>41306</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -455,49 +516,39 @@
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>42064</v>
+        <v>40909</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>42705</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>23</v>
-      </c>
+        <v>41306</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>41306</v>
+        <v>39114</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>42036</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>27</v>
-      </c>
+        <v>40909</v>
+      </c>
+      <c r="G4" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -515,72 +566,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="206.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="186.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="260.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="127.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="172.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">positions!D$2</f>
+        <v>MSD Capital, L.P.</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">positions!D$2</f>
+        <v>MSD Capital, L.P.</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">positions!D$3</f>
+        <v>Promontory Financial Group</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">positions!D$4</f>
+        <v>RR Donnelley</v>
       </c>
     </row>
   </sheetData>
@@ -613,15 +726,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5</v>
@@ -629,7 +742,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -637,7 +750,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -645,7 +758,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.5</v>
@@ -653,7 +766,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4.5</v>
@@ -661,7 +774,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3.5</v>
@@ -669,7 +782,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3</v>
@@ -677,7 +790,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Updated data processing for background processing.
Updated data processing for background processing.
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t xml:space="preserve">in_resume</t>
   </si>
@@ -115,6 +115,12 @@
     <t xml:space="preserve">RR Donnelley</t>
   </si>
   <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overview</t>
+  </si>
+  <si>
     <t xml:space="preserve">detail_1</t>
   </si>
   <si>
@@ -136,6 +142,9 @@
     <t xml:space="preserve">Analytics Platform</t>
   </si>
   <si>
+    <t xml:space="preserve">Msd 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lead development effort on our in-house proprietary data analytics  and risk system on a team of five.</t>
   </si>
   <si>
@@ -157,6 +166,9 @@
     <t xml:space="preserve">Option Pricing Framework</t>
   </si>
   <si>
+    <t xml:space="preserve">trading</t>
+  </si>
+  <si>
     <t xml:space="preserve">Developed a custom in-house option-pricing framework that involved leveraging QuantLib (an open source C++ financial library) for the derivative pricing engine and adding functionality that generated a variance/underlying "shock matrix" for a given option.</t>
   </si>
   <si>
@@ -172,10 +184,19 @@
     <t xml:space="preserve">Independent Foreclosure Review</t>
   </si>
   <si>
-    <t xml:space="preserve">detail</t>
+    <t xml:space="preserve">fa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mortgage review</t>
   </si>
   <si>
     <t xml:space="preserve">RightContent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web App</t>
   </si>
   <si>
     <t xml:space="preserve">skill</t>
@@ -223,6 +244,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,7 +352,7 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -339,7 +361,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="68.4"/>
@@ -447,18 +469,18 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="164.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="55.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="168.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="87.3"/>
@@ -505,7 +527,9 @@
       <c r="E2" s="3" t="n">
         <v>41306</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="n">
+        <v>43800</v>
+      </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,7 +577,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -568,20 +592,20 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="206.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="186.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="206.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="186.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="260.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="127.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="127.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="172.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
@@ -591,115 +615,133 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="0" t="str">
+      <c r="B2" s="0" t="str">
         <f aca="false">positions!D$2</f>
         <v>MSD Capital, L.P.</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="E2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="0" t="str">
+      <c r="B3" s="0" t="str">
         <f aca="false">positions!D$2</f>
         <v>MSD Capital, L.P.</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="0" t="str">
+      <c r="B4" s="0" t="str">
         <f aca="false">positions!D$3</f>
         <v>Promontory Financial Group</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="E4" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="0" t="str">
+      <c r="A5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="str">
         <f aca="false">positions!D$4</f>
         <v>RR Donnelley</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -714,7 +756,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -726,15 +768,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5</v>
@@ -742,7 +784,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -750,7 +792,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -758,7 +800,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.5</v>
@@ -766,7 +808,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4.5</v>
@@ -774,7 +816,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3.5</v>
@@ -782,7 +824,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3</v>
@@ -790,7 +832,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -799,7 +841,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updates to data parsing (role -> projects -> details)
Updates to data parsing (role -> projects -> details)
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,7 +570,7 @@
         <v>39114</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>40909</v>
+        <v>40878</v>
       </c>
       <c r="G4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated layout / background info
layout parsing (support multiple sections), detailed out some more background.
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -12,6 +12,7 @@
     <sheet name="positions" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="projects" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="skills" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="certifications" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t xml:space="preserve">in_resume</t>
   </si>
@@ -82,7 +83,7 @@
     <t xml:space="preserve">Cullowhee, NC</t>
   </si>
   <si>
-    <t xml:space="preserve">Something smart.</t>
+    <t xml:space="preserve">Developed an interactive modeling application using Direct3D for biometric data captured using WISDOM (**W**eakly **I**dentifying **S**ystem for **D**oorway **M**onitoring).</t>
   </si>
   <si>
     <t xml:space="preserve">summary</t>
@@ -97,6 +98,12 @@
     <t xml:space="preserve">MSD Capital, L.P.</t>
   </si>
   <si>
+    <t xml:space="preserve">Managed the software development team, reporting to Chief Operating Officer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSD Capital, L.P. (Cont.)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantitative Developer</t>
   </si>
   <si>
@@ -106,6 +113,9 @@
     <t xml:space="preserve">Promontory Financial Group</t>
   </si>
   <si>
+    <t xml:space="preserve">Software consultant focused on client record auditing systems.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Senior Developer</t>
   </si>
   <si>
@@ -115,6 +125,9 @@
     <t xml:space="preserve">RR Donnelley</t>
   </si>
   <si>
+    <t xml:space="preserve">Web architect for financial publishing and content management applications.</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -142,49 +155,95 @@
     <t xml:space="preserve">Analytics Platform</t>
   </si>
   <si>
-    <t xml:space="preserve">Msd 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead development effort on our in-house proprietary data analytics  and risk system on a team of five.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentation layer constructed with WPF/C#, Service-Oriented-Architecture built with WCF/C#, data layer modeled in T-SQL and processed with R packages deployed to the server instance, invoked directly with stored procedures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Built a suite of FX hedging and settlement tools to automate our FX process. Constructed the core FX Hedging model in R, which used various metrics of hedging (FMV, Cost, MTM, Fixed, Underlying, Custom Model, etc.) to calculate the target hedge by strategy then aggregate by total currency exposure across the firm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build multiple factor-based models in R leveraging Bloomberg data for the India market working directly with the portfolio manager through various iterations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Built a real-time Profit-Loss system by integrating data from our core accounting / OMS systems, then enriching the data sets with market data using our proprietary Market Data service build in WCF using RX/C#.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R, C#, WPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option Pricing Framework</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Developed a custom in-house option-pricing framework that involved leveraging QuantLib (an open source C++ financial library) for the derivative pricing engine and adding functionality that generated a variance/underlying "shock matrix" for a given option.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Developed a WPF application style with a custom configurable n x m matrix data layout (for the pricing matrix), along with custom data overlays in each cell when pricing a strategy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Developed a reusable Bloomberg Data Module for the SAPI API that was responsible for pulling option-pricing parameters (underlying, strike, volatility, maturity date, risk-free rate and dividend yield) in real-time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++, C#, WPF</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lead development </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">effort </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">on a team of five to build our in-house data analytics system.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Collaborated with front office users to develop specifications for predefined and ad-hoc reporting modules (e.g., attribution, exposure, liquidity and cash availability).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked with portfolio managers and analysis to build factor-based models and stock screeners.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed scalable back-end data architecture that leveraged machine learning server (RevoScaleR) to host and execute our internally developed R packages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensured 85%+ unit test coverage over all layers of the application with a combination of NUnit, Moq, tSQL-t and test.that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented a third party data warehouse solution to integrate our accounting, order management and market data systems to streamline the end of day NAV/P&amp;L reporting workflow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R, C#, T-SQL, tidyverse, WPF/WCF, Machine Learning Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trading &amp; Risk Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked with trading and operations to build out a risk management system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created a suite of FX hedging and settlement tools to automate our FX process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Built core hedging model in R to support usage of various hedging metrics (e.g., FMV, MTM, cost, fixed, underlying, custom model) to calculate the target exposure by strategy, then aggregated across the firm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidated disperse analyst models used to build option strategies in Matlab/Excel into an application framework built by leveraging QuantLib.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Built a real-time profit-loss system by integrating data from our core accounting / OMS systems and enriching it with market data using our market data service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed a reusable market data service that encapsulated real-time feed requests for dependent upstream applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R, C++, C#, WPF/WCF, ReactiveX, QuantLib, Bloomberg SAPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked with research analysts to create a global repository of company research.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed a non-intrusive metadata tagging system used to tag and identify research content.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used supervised learning methods to automatically tag user generated and external content (e.g., company, filing, write-up, model, earnings call).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python, CLI/C++ Interop, NLP</t>
   </si>
   <si>
     <t xml:space="preserve">Independent Foreclosure Review</t>
   </si>
   <si>
-    <t xml:space="preserve">fa</t>
+    <t xml:space="preserve">Lead development and implementation on workflow application designed to audit fortune 10 client.</t>
   </si>
   <si>
     <t xml:space="preserve">mortgage review</t>
@@ -227,6 +286,18 @@
   </si>
   <si>
     <t xml:space="preserve">SAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantitative Analyst with R Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataCamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.datacamp.com/statement-of-accomplishment/track/fa7e06dfeb137b96429de33fba1fec46946019b8</t>
   </si>
 </sst>
 </file>
@@ -239,7 +310,7 @@
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -260,6 +331,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -304,7 +387,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,8 +412,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -352,8 +447,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,8 +459,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="68.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="65.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="122.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="66.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="44.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
@@ -467,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,7 +576,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="55.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="68.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="168.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="87.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="75.62"/>
@@ -530,49 +625,76 @@
       <c r="F2" s="3" t="n">
         <v>43800</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="E3" s="3" t="n">
-        <v>40909</v>
+        <v>41307</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>41306</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>43801</v>
+      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="3" t="n">
+        <v>40909</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>41306</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="3" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>39114</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F5" s="3" t="n">
         <v>40878</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -590,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,13 +723,14 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="84.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="206.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="186.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="260.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="127.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="172.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="131.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="184.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,31 +741,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -651,28 +774,28 @@
         <v>MSD Capital, L.P.</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,58 +807,87 @@
         <v>MSD Capital, L.P.</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="str">
-        <f aca="false">positions!D$3</f>
-        <v>Promontory Financial Group</v>
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="b">
-        <v>1</v>
+      <c r="A5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="str">
         <f aca="false">positions!D$4</f>
+        <v>Promontory Financial Group</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">positions!D$5</f>
         <v>RR Donnelley</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>57</v>
+      <c r="C6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +909,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -768,15 +920,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5</v>
@@ -784,7 +936,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -792,7 +944,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -800,7 +952,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.5</v>
@@ -808,7 +960,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4.5</v>
@@ -816,7 +968,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3.5</v>
@@ -824,7 +976,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3</v>
@@ -832,7 +984,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -847,4 +999,66 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="88.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.datacamp.com/statement-of-accomplishment/track/fa7e06dfeb137b96429de33fba1fec46946019b8"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to formatting & background data.
Background info, certs section, parsing.
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
   <si>
     <t xml:space="preserve">in_resume</t>
   </si>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">Promontory Financial Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Software consultant focused on client record auditing systems.</t>
+    <t xml:space="preserve">On-site and remote software consultant focused on client record auditing systems.</t>
   </si>
   <si>
     <t xml:space="preserve">Senior Developer</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">RR Donnelley</t>
   </si>
   <si>
-    <t xml:space="preserve">Web architect for financial publishing and content management applications.</t>
+    <t xml:space="preserve">Technical architect for financial publishing and content management applications.</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -246,16 +246,37 @@
     <t xml:space="preserve">Lead development and implementation on workflow application designed to audit fortune 10 client.</t>
   </si>
   <si>
-    <t xml:space="preserve">mortgage review</t>
+    <t xml:space="preserve">Managed client deliverables with an average development life-cycle of 2.5 weeks throughout the project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System concurrently supported 2,000+ users in the system with an average transaction count of 1.1 million per day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The resulting data set was used as the statistical basis for agreed financial settlement to borrowers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assisted SMEs in converting legacy SAS models to R and validating statistical output.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C#, T-SQL, R, SAS, WPF, Full-text Index</t>
   </si>
   <si>
     <t xml:space="preserve">RightContent</t>
   </si>
   <si>
-    <t xml:space="preserve">fsad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web App</t>
+    <t xml:space="preserve">Technical architect for a suite of financial publishing applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented the full specification for front-page server extensions (version 13.1) to enable native (i.e., Word, Excel) remote content authoring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrote a comprehensive functional language that enabled an expression syntax SMEs used to migrate content between platforms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed an LL parsering engine and supporting libraries for content transformation and styling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C#, T-SQL, ASP.NET, WebDAV</t>
   </si>
   <si>
     <t xml:space="preserve">skill</t>
@@ -288,16 +309,34 @@
     <t xml:space="preserve">SAS</t>
   </si>
   <si>
+    <t xml:space="preserve">when</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
     <t xml:space="preserve">link</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantitative Analyst with R Track</t>
+    <t xml:space="preserve">Quantitative Analyst with R</t>
   </si>
   <si>
     <t xml:space="preserve">DataCamp</t>
   </si>
   <si>
+    <t xml:space="preserve">Certification</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.datacamp.com/statement-of-accomplishment/track/fa7e06dfeb137b96429de33fba1fec46946019b8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mathematics for Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imperial College London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.coursera.org/account/accomplishments/specialization/certificate/SUFEV6B5JVAN</t>
   </si>
 </sst>
 </file>
@@ -310,7 +349,7 @@
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -336,6 +375,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -387,7 +431,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,12 +464,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -564,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -576,7 +628,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="68.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="69.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="168.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="87.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="75.62"/>
@@ -623,7 +675,7 @@
         <v>41306</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>43800</v>
+        <v>43739</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
@@ -646,7 +698,7 @@
         <v>41307</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>43801</v>
+        <v>43739</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -714,8 +766,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,7 +781,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="260.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="131.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="184.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="59.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -854,7 +906,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -871,8 +923,20 @@
       <c r="E5" s="0" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -881,13 +945,22 @@
         <v>RR Donnelley</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -920,15 +993,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5</v>
@@ -936,7 +1009,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -944,7 +1017,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -952,7 +1025,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.5</v>
@@ -960,7 +1033,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4.5</v>
@@ -968,7 +1041,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3.5</v>
@@ -976,7 +1049,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>3</v>
@@ -984,7 +1057,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -1006,19 +1079,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="88.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="88.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,26 +1107,61 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="b">
+      <c r="A2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>42005</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>43800</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.datacamp.com/statement-of-accomplishment/track/fa7e06dfeb137b96429de33fba1fec46946019b8"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.datacamp.com/statement-of-accomplishment/track/fa7e06dfeb137b96429de33fba1fec46946019b8"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.coursera.org/account/accomplishments/specialization/certificate/SUFEV6B5JVAN"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Tweaks to background & formatting.
Tweaks to background & formatting.
</commit_message>
<xml_diff>
--- a/background.xlsx
+++ b/background.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" state="visible" r:id="rId2"/>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">Emphasis on both supervised and unsupervised statistical learning techniques.</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial engineering and risk analytics as electives.</t>
-  </si>
-  <si>
     <t xml:space="preserve">B.S., Computer Science (minor Mathematics)</t>
   </si>
   <si>
@@ -155,32 +152,7 @@
     <t xml:space="preserve">Analytics Platform</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lead development </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">effort </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">on a team of five to build our in-house data analytics system.</t>
-    </r>
+    <t xml:space="preserve">Lead development effort on a team of five to build our in-house data analytics system.</t>
   </si>
   <si>
     <t xml:space="preserve">Collaborated with front office users to develop specifications for predefined and ad-hoc reporting modules (e.g., attribution, exposure, liquidity and cash availability).</t>
@@ -195,7 +167,7 @@
     <t xml:space="preserve">Ensured 85%+ unit test coverage over all layers of the application with a combination of NUnit, Moq, tSQL-t and test.that.</t>
   </si>
   <si>
-    <t xml:space="preserve">Implemented a third party data warehouse solution to integrate our accounting, order management and market data systems to streamline the end of day NAV/P&amp;L reporting workflow.</t>
+    <t xml:space="preserve">Implemented a third party data warehouse solution to integrate accounting and order management systems to streamline the end of day NAV/P&amp;L reporting.</t>
   </si>
   <si>
     <t xml:space="preserve">R, C#, T-SQL, tidyverse, WPF/WCF, Machine Learning Server</t>
@@ -235,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">Used supervised learning methods to automatically tag user generated and external content (e.g., company, filing, write-up, model, earnings call).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research content automatically parsed for investment indicators (i.e., price targets) and stored in elasticsearch.</t>
   </si>
   <si>
     <t xml:space="preserve">Python, CLI/C++ Interop, NLP</t>
@@ -349,7 +324,7 @@
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -374,12 +349,8 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -431,7 +402,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -464,19 +435,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,8 +466,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -571,22 +538,19 @@
       <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>38200</v>
@@ -595,7 +559,7 @@
         <v>39052</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +580,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -655,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,13 +627,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>41306</v>
@@ -678,7 +642,7 @@
         <v>43739</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,13 +650,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>41307</v>
@@ -707,13 +671,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>40909</v>
@@ -722,7 +686,7 @@
         <v>41306</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,13 +694,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>39114</v>
@@ -745,7 +709,7 @@
         <v>40878</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -766,8 +730,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,28 +757,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,28 +790,28 @@
         <v>MSD Capital, L.P.</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,47 +823,50 @@
         <v>MSD Capital, L.P.</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>25</v>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>61</v>
       </c>
       <c r="J4" s="0" t="s">
@@ -929,7 +896,7 @@
       <c r="G5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>68</v>
       </c>
       <c r="J5" s="0" t="s">
@@ -1082,7 +1049,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1101,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -1117,7 +1084,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="b">
+      <c r="A2" s="8" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1132,14 +1099,14 @@
       <c r="E2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="b">
+      <c r="A3" s="8" t="b">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -1154,7 +1121,7 @@
       <c r="E3" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>